<commit_message>
Created topic plots and cleaned up code.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mutej\Desktop\homework\network\IS527-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDEE8CAC-888B-4C20-9DB8-B649B30F0B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F82CE2-E031-4D46-8CD3-5A49C8A9B40C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4130" yWindow="570" windowWidth="12330" windowHeight="9300" xr2:uid="{739E577A-96C2-4651-A768-334F2AA90105}"/>
+    <workbookView xWindow="4470" yWindow="900" windowWidth="12330" windowHeight="9300" activeTab="1" xr2:uid="{739E577A-96C2-4651-A768-334F2AA90105}"/>
   </bookViews>
   <sheets>
     <sheet name="episode6" sheetId="8" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2064" uniqueCount="664">
   <si>
     <t>PAULA</t>
   </si>
@@ -1618,9 +1618,6 @@
   </si>
   <si>
     <t xml:space="preserve">Hi. What’s up?  Now is the time.  Now?  We’re going on a dive boat. We leave the dock at 3:00.  She’s not gonna bring her jewelry with her on the boat.  Look, I– I don’t know about this, Paula.  Just one of those bracelets, just one, is worth 75,000 dollars.  Kai, think what you can do with that.  You know, you could finally hire a good lawyer to fight these fuckers.  Oh, shit. Paula, I–  You can help your brothers.  They won’t give you shit for taking this job, that’s for sure, not after the way you come through for them like this.  I just– I don’t– I don’t– I don’t steal from people, you know?  They stole from you.  They stole all of this from you. You know that.  But it’s different. It’s– It’s different people.  No, they’re the same people. They’re all the same people.  Don’t you see they’re all the same people?  All of these people, at some point, have stolen from someone like you.  And they don’t need it. They won’t even miss it.  They have all this money, and they don’t even know what to do with it.  And then there’s someone like you who’s struggling.  I know, but–  That’s not right.  I agree. But I just– Aren’t these people, like, your friends? Like–  They’re not my friends.  No, they’re not my friends.  Holy shit, Paula, I don’t know.  We leave the hotel Thursday and there might not be a better time than now.  You still have that master key, right?  So it’ll get you into our suite? Yeah.  The code to the safe is 1026.  It’ll be easy.  And you can finally get the money to fight and get back everything that was stolen from you.  Look, you can do what you want, but at 3:00 p.m., the suite will be empty.  Okay. Thanks. </t>
-  </si>
-  <si>
-    <t>RACHEL’S MOM</t>
   </si>
   <si>
     <t>Hello?  Hi, Mom.  Hey, Rach, how are you? You guys having fun?  I don’t know. I’m just having–  Um, I don’t–  What is it?  Um– I don’t know. Um, I just– I feel like– I’m thinking that this isn’t–  It’s hard to hear you, sweetie.  I just got to the market. Can I call you when I get home?  Yeah. Yeah, of course.  Yeah, just call me later. Okay. I love you, Mom.  Yeah, I’m gonna call you later.  I love you.  Okay, love you.  Love you.  I’ll try you from the car.  Bye.</t>
@@ -2397,7 +2394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02F47D4C-C53C-4FA5-8E03-CD7C20E05B9B}">
   <dimension ref="A1:C108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+    <sheetView topLeftCell="A55" workbookViewId="0">
       <selection activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
@@ -2416,13 +2413,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
@@ -2433,18 +2430,18 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="B4" t="s">
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
@@ -2455,7 +2452,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
@@ -2466,7 +2463,7 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
@@ -2477,7 +2474,7 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
@@ -2488,7 +2485,7 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
@@ -2499,7 +2496,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
@@ -2521,7 +2518,7 @@
         <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
@@ -2532,7 +2529,7 @@
         <v>2</v>
       </c>
       <c r="C12" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -2543,7 +2540,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
@@ -2554,7 +2551,7 @@
         <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -2565,7 +2562,7 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
@@ -2598,7 +2595,7 @@
         <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -2609,7 +2606,7 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
@@ -2620,7 +2617,7 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -2642,7 +2639,7 @@
         <v>3</v>
       </c>
       <c r="C22" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
@@ -2653,7 +2650,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
@@ -2664,7 +2661,7 @@
         <v>9</v>
       </c>
       <c r="C24" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
@@ -2675,7 +2672,7 @@
         <v>9</v>
       </c>
       <c r="C25" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
@@ -2686,7 +2683,7 @@
         <v>9</v>
       </c>
       <c r="C26" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
@@ -2697,7 +2694,7 @@
         <v>9</v>
       </c>
       <c r="C27" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.35">
@@ -2708,7 +2705,7 @@
         <v>9</v>
       </c>
       <c r="C28" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.35">
@@ -2719,7 +2716,7 @@
         <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
@@ -2730,7 +2727,7 @@
         <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
@@ -2741,7 +2738,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
@@ -2752,7 +2749,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
@@ -2763,7 +2760,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
@@ -2774,7 +2771,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.35">
@@ -2785,7 +2782,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
@@ -2796,7 +2793,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
@@ -2807,7 +2804,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
@@ -2818,7 +2815,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
@@ -2829,7 +2826,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
@@ -2840,7 +2837,7 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
@@ -2851,7 +2848,7 @@
         <v>9</v>
       </c>
       <c r="C41" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
@@ -2862,7 +2859,7 @@
         <v>17</v>
       </c>
       <c r="C42" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
@@ -2873,7 +2870,7 @@
         <v>4</v>
       </c>
       <c r="C43" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
@@ -2884,7 +2881,7 @@
         <v>2</v>
       </c>
       <c r="C44" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
@@ -2895,7 +2892,7 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
@@ -2906,7 +2903,7 @@
         <v>3</v>
       </c>
       <c r="C46" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
@@ -2917,7 +2914,7 @@
         <v>3</v>
       </c>
       <c r="C47" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
@@ -2928,7 +2925,7 @@
         <v>2</v>
       </c>
       <c r="C48" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
@@ -2939,7 +2936,7 @@
         <v>6</v>
       </c>
       <c r="C49" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
@@ -2950,7 +2947,7 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.35">
@@ -2961,7 +2958,7 @@
         <v>3</v>
       </c>
       <c r="C51" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.35">
@@ -2972,7 +2969,7 @@
         <v>3</v>
       </c>
       <c r="C52" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.35">
@@ -2983,7 +2980,7 @@
         <v>2</v>
       </c>
       <c r="C53" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.35">
@@ -2994,7 +2991,7 @@
         <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.35">
@@ -3016,18 +3013,18 @@
         <v>3</v>
       </c>
       <c r="C56" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B57" t="s">
         <v>10</v>
       </c>
       <c r="C57" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.35">
@@ -3038,7 +3035,7 @@
         <v>10</v>
       </c>
       <c r="C58" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.35">
@@ -3049,7 +3046,7 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.35">
@@ -3060,7 +3057,7 @@
         <v>1</v>
       </c>
       <c r="C60" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.35">
@@ -3071,7 +3068,7 @@
         <v>2</v>
       </c>
       <c r="C61" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.35">
@@ -3082,7 +3079,7 @@
         <v>2</v>
       </c>
       <c r="C62" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.35">
@@ -3093,7 +3090,7 @@
         <v>2</v>
       </c>
       <c r="C63" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.35">
@@ -3104,7 +3101,7 @@
         <v>2</v>
       </c>
       <c r="C64" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
@@ -3115,7 +3112,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
@@ -3126,7 +3123,7 @@
         <v>221</v>
       </c>
       <c r="C66" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -3137,7 +3134,7 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -3148,7 +3145,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -3159,18 +3156,18 @@
         <v>4</v>
       </c>
       <c r="C69" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
+        <v>627</v>
+      </c>
+      <c r="B70" t="s">
+        <v>3</v>
+      </c>
+      <c r="C70" t="s">
         <v>628</v>
-      </c>
-      <c r="B70" t="s">
-        <v>3</v>
-      </c>
-      <c r="C70" t="s">
-        <v>629</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -3181,7 +3178,7 @@
         <v>13</v>
       </c>
       <c r="C71" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -3192,7 +3189,7 @@
         <v>3</v>
       </c>
       <c r="C72" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -3203,7 +3200,7 @@
         <v>7</v>
       </c>
       <c r="C73" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -3214,7 +3211,7 @@
         <v>0</v>
       </c>
       <c r="C74" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -3225,7 +3222,7 @@
         <v>1</v>
       </c>
       <c r="C75" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -3236,7 +3233,7 @@
         <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -3247,7 +3244,7 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -3258,7 +3255,7 @@
         <v>0</v>
       </c>
       <c r="C78" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -3269,7 +3266,7 @@
         <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -3280,7 +3277,7 @@
         <v>0</v>
       </c>
       <c r="C80" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -3291,7 +3288,7 @@
         <v>1</v>
       </c>
       <c r="C81" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -3302,7 +3299,7 @@
         <v>5</v>
       </c>
       <c r="C82" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -3313,7 +3310,7 @@
         <v>7</v>
       </c>
       <c r="C83" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -3324,7 +3321,7 @@
         <v>4</v>
       </c>
       <c r="C84" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -3335,7 +3332,7 @@
         <v>2</v>
       </c>
       <c r="C85" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -3346,7 +3343,7 @@
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -3357,7 +3354,7 @@
         <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -3368,7 +3365,7 @@
         <v>2</v>
       </c>
       <c r="C88" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -3379,7 +3376,7 @@
         <v>2</v>
       </c>
       <c r="C89" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -3390,7 +3387,7 @@
         <v>6</v>
       </c>
       <c r="C90" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -3401,7 +3398,7 @@
         <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -3412,7 +3409,7 @@
         <v>6</v>
       </c>
       <c r="C92" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -3423,7 +3420,7 @@
         <v>2</v>
       </c>
       <c r="C93" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -3434,7 +3431,7 @@
         <v>4</v>
       </c>
       <c r="C94" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -3445,7 +3442,7 @@
         <v>7</v>
       </c>
       <c r="C95" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -3456,7 +3453,7 @@
         <v>18</v>
       </c>
       <c r="C96" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -3467,7 +3464,7 @@
         <v>18</v>
       </c>
       <c r="C97" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -3478,7 +3475,7 @@
         <v>7</v>
       </c>
       <c r="C98" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -3489,7 +3486,7 @@
         <v>18</v>
       </c>
       <c r="C99" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -3500,7 +3497,7 @@
         <v>15</v>
       </c>
       <c r="C100" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -3511,7 +3508,7 @@
         <v>23</v>
       </c>
       <c r="C101" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -3522,7 +3519,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -3533,7 +3530,7 @@
         <v>1</v>
       </c>
       <c r="C103" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -3544,7 +3541,7 @@
         <v>5</v>
       </c>
       <c r="C104" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -3555,7 +3552,7 @@
         <v>9</v>
       </c>
       <c r="C105" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -3563,10 +3560,10 @@
         <v>9</v>
       </c>
       <c r="B106" t="s">
+        <v>660</v>
+      </c>
+      <c r="C106" t="s">
         <v>661</v>
-      </c>
-      <c r="C106" t="s">
-        <v>662</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -3577,7 +3574,7 @@
         <v>3</v>
       </c>
       <c r="C107" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -3588,7 +3585,7 @@
         <v>9</v>
       </c>
       <c r="C108" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -3600,8 +3597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8735F112-8041-4E4A-B9F2-920EF24E7491}">
   <dimension ref="A1:C112"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4323,13 +4320,13 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
+        <v>280</v>
+      </c>
+      <c r="B66" t="s">
+        <v>4</v>
+      </c>
+      <c r="C66" t="s">
         <v>525</v>
-      </c>
-      <c r="B66" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>526</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.35">
@@ -4340,7 +4337,7 @@
         <v>4</v>
       </c>
       <c r="C67" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
@@ -4351,7 +4348,7 @@
         <v>2</v>
       </c>
       <c r="C68" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
@@ -4362,7 +4359,7 @@
         <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
@@ -4373,7 +4370,7 @@
         <v>2</v>
       </c>
       <c r="C70" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
@@ -4384,7 +4381,7 @@
         <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
@@ -4395,7 +4392,7 @@
         <v>6</v>
       </c>
       <c r="C72" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
@@ -4406,7 +4403,7 @@
         <v>6</v>
       </c>
       <c r="C73" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
@@ -4417,7 +4414,7 @@
         <v>18</v>
       </c>
       <c r="C74" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
@@ -4428,7 +4425,7 @@
         <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
@@ -4439,7 +4436,7 @@
         <v>22</v>
       </c>
       <c r="C76" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
@@ -4450,7 +4447,7 @@
         <v>6</v>
       </c>
       <c r="C77" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
@@ -4461,7 +4458,7 @@
         <v>22</v>
       </c>
       <c r="C78" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
@@ -4472,7 +4469,7 @@
         <v>13</v>
       </c>
       <c r="C79" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
@@ -4483,7 +4480,7 @@
         <v>1</v>
       </c>
       <c r="C80" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
@@ -4494,7 +4491,7 @@
         <v>10</v>
       </c>
       <c r="C81" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
@@ -4505,7 +4502,7 @@
         <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
@@ -4516,7 +4513,7 @@
         <v>10</v>
       </c>
       <c r="C83" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
@@ -4527,7 +4524,7 @@
         <v>2</v>
       </c>
       <c r="C84" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
@@ -4538,7 +4535,7 @@
         <v>3</v>
       </c>
       <c r="C85" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
@@ -4549,7 +4546,7 @@
         <v>3</v>
       </c>
       <c r="C86" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
@@ -4560,7 +4557,7 @@
         <v>6</v>
       </c>
       <c r="C87" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
@@ -4571,7 +4568,7 @@
         <v>3</v>
       </c>
       <c r="C88" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
@@ -4582,7 +4579,7 @@
         <v>6</v>
       </c>
       <c r="C89" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
@@ -4593,7 +4590,7 @@
         <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
@@ -4604,7 +4601,7 @@
         <v>6</v>
       </c>
       <c r="C91" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
@@ -4615,7 +4612,7 @@
         <v>9</v>
       </c>
       <c r="C92" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
@@ -4626,7 +4623,7 @@
         <v>4</v>
       </c>
       <c r="C93" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
@@ -4637,7 +4634,7 @@
         <v>9</v>
       </c>
       <c r="C94" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
@@ -4648,7 +4645,7 @@
         <v>23</v>
       </c>
       <c r="C95" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
@@ -4659,7 +4656,7 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
@@ -4670,7 +4667,7 @@
         <v>6</v>
       </c>
       <c r="C97" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
@@ -4681,7 +4678,7 @@
         <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
@@ -4692,7 +4689,7 @@
         <v>9</v>
       </c>
       <c r="C99" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
@@ -4703,7 +4700,7 @@
         <v>4</v>
       </c>
       <c r="C100" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
@@ -4714,7 +4711,7 @@
         <v>9</v>
       </c>
       <c r="C101" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
@@ -4725,7 +4722,7 @@
         <v>4</v>
       </c>
       <c r="C102" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
@@ -4736,7 +4733,7 @@
         <v>9</v>
       </c>
       <c r="C103" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
@@ -4747,7 +4744,7 @@
         <v>4</v>
       </c>
       <c r="C104" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
@@ -4758,7 +4755,7 @@
         <v>16</v>
       </c>
       <c r="C105" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
@@ -4769,7 +4766,7 @@
         <v>9</v>
       </c>
       <c r="C106" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
@@ -4780,7 +4777,7 @@
         <v>4</v>
       </c>
       <c r="C107" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
@@ -4791,7 +4788,7 @@
         <v>23</v>
       </c>
       <c r="C108" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
@@ -4802,7 +4799,7 @@
         <v>2</v>
       </c>
       <c r="C109" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
@@ -4813,7 +4810,7 @@
         <v>5</v>
       </c>
       <c r="C110" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
@@ -4824,7 +4821,7 @@
         <v>9</v>
       </c>
       <c r="C111" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
@@ -4835,7 +4832,7 @@
         <v>0</v>
       </c>
       <c r="C112" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
   </sheetData>

</xml_diff>